<commit_message>
process run recording completed
</commit_message>
<xml_diff>
--- a/soberano/test_cases/inventory_operation_preconditions_test_cases.xlsx
+++ b/soberano/test_cases/inventory_operation_preconditions_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t xml:space="preserve">After material expenses recording test cases, this is the expected global (all warehouses) stock.</t>
   </si>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">Authorized user1</t>
   </si>
   <si>
-    <t xml:space="preserve">mprov1</t>
+    <t xml:space="preserve">mprov2</t>
   </si>
   <si>
     <t xml:space="preserve">mc2</t>
@@ -109,19 +109,10 @@
     <t xml:space="preserve">Authorized user2</t>
   </si>
   <si>
-    <t xml:space="preserve">mprov2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Authorized user3</t>
   </si>
   <si>
-    <t xml:space="preserve">mprov3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Authorized user4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mprov4</t>
   </si>
   <si>
     <t xml:space="preserve">After running the above tests, this is the expected global (all warehouses) stock.</t>
@@ -207,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,14 +212,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,10 +239,10 @@
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.25"/>
@@ -390,10 +373,10 @@
       <c r="I10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -425,10 +408,10 @@
       <c r="I11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="5" t="s">
+      <c r="J11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -440,7 +423,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>8</v>
@@ -461,10 +444,10 @@
       <c r="I12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" s="5" t="s">
+      <c r="J12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -473,10 +456,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>10</v>
@@ -497,10 +480,10 @@
       <c r="I13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" s="5" t="s">
+      <c r="J13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -509,10 +492,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
@@ -533,10 +516,10 @@
       <c r="I14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K14" s="5" t="s">
+      <c r="J14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -545,7 +528,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -645,14 +628,14 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="6"/>
+      <c r="B26" s="4"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="6"/>
+      <c r="B28" s="4"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
specifying inventory recalculation test cases in progress
</commit_message>
<xml_diff>
--- a/soberano/test_cases/inventory_operation_preconditions_test_cases.xlsx
+++ b/soberano/test_cases/inventory_operation_preconditions_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t xml:space="preserve">After material expenses recording test cases, this is the expected global (all warehouses) stock.</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Days before current day</t>
   </si>
   <si>
     <t xml:space="preserve">Provider</t>
@@ -126,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -155,6 +158,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -198,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +221,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,20 +252,20 @@
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="35.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="35.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,7 +291,7 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AMI4" s="0"/>
+      <c r="E4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,14 +365,14 @@
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>17</v>
@@ -378,6 +391,9 @@
       </c>
       <c r="K10" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,34 +401,37 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>-1</v>
+      </c>
       <c r="D11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="F11" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="H11" s="2" t="n">
         <v>2000</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>27</v>
+      <c r="K11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,35 +439,38 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>-1</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="F12" s="2" t="n">
         <f aca="false">B6</f>
         <v>1360776000000</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="H12" s="2" t="n">
         <v>300000000000000</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>27</v>
+      <c r="K12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,35 +478,38 @@
         <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>-1</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="F13" s="2" t="n">
         <f aca="false">B7</f>
         <v>1360776002001</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="H13" s="2" t="n">
         <v>800000000000000</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>27</v>
+      <c r="K13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,54 +517,57 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">B8</f>
         <v>1000.001</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="H14" s="2" t="n">
         <v>500000</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>27</v>
+      <c r="K14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -548,13 +576,12 @@
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,14 +589,15 @@
         <v>6</v>
       </c>
       <c r="B20" s="2" t="n">
-        <f aca="false">B5+E11</f>
+        <f aca="false">B5+F11</f>
         <v>1907.184000002</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="3" t="n">
-        <f aca="false">(B5*D5+G11)/(B5+E11)</f>
+      <c r="E20" s="3" t="n">
+        <f aca="false">(B5*D5+H11)/(B5+F11)</f>
         <v>8409.79961555056</v>
       </c>
     </row>
@@ -578,14 +606,15 @@
         <v>8</v>
       </c>
       <c r="B21" s="2" t="n">
-        <f aca="false">B6+E12</f>
+        <f aca="false">B6+F12</f>
         <v>2721552000000</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="3" t="n">
-        <f aca="false">(B6*D6+G12)/(B6+E12)</f>
+      <c r="E21" s="3" t="n">
+        <f aca="false">(B6*D6+H12)/(B6+F12)</f>
         <v>110.231221009189</v>
       </c>
     </row>
@@ -594,14 +623,15 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="n">
-        <f aca="false">B7+E13</f>
+        <f aca="false">B7+F13</f>
         <v>2721552004002</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="3" t="n">
-        <f aca="false">(B7*D7+G13)/(B7+E13)</f>
+      <c r="E22" s="3" t="n">
+        <f aca="false">(B7*D7+H13)/(B7+F13)</f>
         <v>293.949922258922</v>
       </c>
     </row>
@@ -610,36 +640,39 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="n">
-        <f aca="false">B8+E14</f>
+        <f aca="false">B8+F14</f>
         <v>2000.002</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="3" t="n">
-        <f aca="false">(B8*D8+G14)/(B8+E14)</f>
+      <c r="E23" s="3" t="n">
+        <f aca="false">(B8*D8+H14)/(B8+F14)</f>
         <v>249.99975000075</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="4"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="4"/>
-      <c r="E28" s="2"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
material expense recording and canceling with inventory recalculation derived from expenses past history change. coding completed. testing in progress.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/inventory_operation_preconditions_test_cases.xlsx
+++ b/soberano/test_cases/inventory_operation_preconditions_test_cases.xlsx
@@ -129,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -158,12 +158,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,10 +215,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,7 +245,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.25"/>
@@ -365,7 +355,7 @@
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -404,7 +394,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>25</v>
@@ -427,10 +417,10 @@
       <c r="J11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="5" t="s">
+      <c r="K11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -442,7 +432,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>25</v>
@@ -466,10 +456,10 @@
       <c r="J12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="5" t="s">
+      <c r="K12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -481,7 +471,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>25</v>
@@ -505,10 +495,10 @@
       <c r="J13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="5" t="s">
+      <c r="K13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -520,7 +510,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>25</v>
@@ -544,10 +534,10 @@
       <c r="J14" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="5" t="s">
+      <c r="K14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -659,16 +649,16 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>